<commit_message>
variable practice - pounds
</commit_message>
<xml_diff>
--- a/raw data - variables.xlsx
+++ b/raw data - variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominicluther/Library/CloudStorage/Dropbox/Coding/JavaScript/programming-inspiration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310B3FB8-B151-F94C-A696-45F8D8B8FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6827CC4-19C3-5647-BCB1-E6EDB247B8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{6B3E97B3-2387-3E4E-B7AF-B8A339706F03}"/>
   </bookViews>
@@ -36,41 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="156">
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Response</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="182">
   <si>
     <t>age</t>
   </si>
   <si>
-    <t>Question1</t>
-  </si>
-  <si>
-    <t>Question2</t>
-  </si>
-  <si>
     <t>Give me a number</t>
   </si>
   <si>
     <t>Give me another number</t>
   </si>
   <si>
-    <t>Answer1</t>
-  </si>
-  <si>
-    <t>Answer2</t>
-  </si>
-  <si>
-    <t>Variable1</t>
-  </si>
-  <si>
-    <t>Variable2</t>
-  </si>
-  <si>
     <t>num1</t>
   </si>
   <si>
@@ -86,39 +62,15 @@
     <t>tell you how old you were last year</t>
   </si>
   <si>
-    <t>Variable3</t>
-  </si>
-  <si>
     <t>result</t>
   </si>
   <si>
-    <t>Last year, you were {result}</t>
-  </si>
-  <si>
-    <t>In 10 years, you will be {result}</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>{answer1} * {answer2} is {result}</t>
-  </si>
-  <si>
     <t>tell you how old you'll be next year</t>
   </si>
   <si>
-    <t>Next year, you'll be {result}</t>
-  </si>
-  <si>
     <t>take one number from the other</t>
   </si>
   <si>
-    <t>{answer1} - {answer2} is {result}</t>
-  </si>
-  <si>
-    <t>{answer1} / {answer2} is {result}</t>
-  </si>
-  <si>
     <t>work out how many pizza slices there are left</t>
   </si>
   <si>
@@ -134,9 +86,6 @@
     <t>How many slices did you eat?</t>
   </si>
   <si>
-    <t>You have {result} slices left</t>
-  </si>
-  <si>
     <t>work out how much each person owes</t>
   </si>
   <si>
@@ -161,21 +110,12 @@
     <t>How heavy is it in pounds?</t>
   </si>
   <si>
-    <t>{answer1} lbs is {result} kg</t>
-  </si>
-  <si>
     <t>tell them how many times a number fits in</t>
   </si>
   <si>
-    <t>There are {result} {answer2}s in {answer1}</t>
-  </si>
-  <si>
     <t>tell them the remainder when dividing</t>
   </si>
   <si>
-    <t>There are {result} left over after dividing {answer1} by {answer2}</t>
-  </si>
-  <si>
     <t>tell them how many hours there are in that many days</t>
   </si>
   <si>
@@ -185,9 +125,6 @@
     <t>Give me a number of hours</t>
   </si>
   <si>
-    <t>There are {result} hours in {answer1} days</t>
-  </si>
-  <si>
     <t>tell someone how long it will take to save their pocket money</t>
   </si>
   <si>
@@ -203,9 +140,6 @@
     <t>How much do you want to save?</t>
   </si>
   <si>
-    <t>It will take {result} weeks to save £{answer1}</t>
-  </si>
-  <si>
     <t>work out how much someone spends on chocolate</t>
   </si>
   <si>
@@ -233,9 +167,6 @@
     <t>How many days is your holiday?</t>
   </si>
   <si>
-    <t>You will have £{result} a day</t>
-  </si>
-  <si>
     <t>divide one number by another</t>
   </si>
   <si>
@@ -245,30 +176,15 @@
     <t>add two numbers together</t>
   </si>
   <si>
-    <t>{answer1} + {answer2} is {result}</t>
-  </si>
-  <si>
     <t>work out how many hours Squidward has practiced</t>
   </si>
   <si>
     <t>hours</t>
   </si>
   <si>
-    <t>How many hours a day?</t>
-  </si>
-  <si>
     <t>For how many days?</t>
   </si>
   <si>
-    <t>Squidward has practiced {result} hours</t>
-  </si>
-  <si>
-    <t>{answer1} chocolate bars is {result}</t>
-  </si>
-  <si>
-    <t>You each owe £{result}</t>
-  </si>
-  <si>
     <t>calculate the area of a rectangle</t>
   </si>
   <si>
@@ -284,9 +200,6 @@
     <t>What's the width of the recatangle?</t>
   </si>
   <si>
-    <t>The area of the rectangle is {result}</t>
-  </si>
-  <si>
     <t>calculate the perimeter of a rectangle</t>
   </si>
   <si>
@@ -299,15 +212,9 @@
     <t>minutes</t>
   </si>
   <si>
-    <t>There are {result} seconds in {answer1} minutes</t>
-  </si>
-  <si>
     <t>calculate the average of two numbers</t>
   </si>
   <si>
-    <t>The average is {result}</t>
-  </si>
-  <si>
     <t>work out the difference in ages</t>
   </si>
   <si>
@@ -323,9 +230,6 @@
     <t>How old is the first person?</t>
   </si>
   <si>
-    <t>Person 1 is {result} years older</t>
-  </si>
-  <si>
     <t>work out how many boxes you need</t>
   </si>
   <si>
@@ -341,9 +245,6 @@
     <t>How many fit in a box?</t>
   </si>
   <si>
-    <t>{answer1} needs {result} boxes</t>
-  </si>
-  <si>
     <t>say how far you have cycled</t>
   </si>
   <si>
@@ -356,48 +257,27 @@
     <t>How many days did you cycle for?</t>
   </si>
   <si>
-    <t>You cycled {result}km in {answer2} days</t>
-  </si>
-  <si>
-    <t>The perimeter of the rectangle is {result}</t>
-  </si>
-  <si>
     <t>the square of a number</t>
   </si>
   <si>
-    <t>{answer1} squared is {result}</t>
-  </si>
-  <si>
     <t>half a number</t>
   </si>
   <si>
-    <t>Half of {answer1} is {result}</t>
-  </si>
-  <si>
     <t>double a number</t>
   </si>
   <si>
-    <t>Double {answer1} is {result}</t>
-  </si>
-  <si>
     <t>area of a square</t>
   </si>
   <si>
     <t>How long is the square?</t>
   </si>
   <si>
-    <t>The square is {result} cm2</t>
-  </si>
-  <si>
     <t>perimeter of a square</t>
   </si>
   <si>
     <t>triple a number</t>
   </si>
   <si>
-    <t>Triple {answer1} is {result}</t>
-  </si>
-  <si>
     <t>convert from celsius to fahrenheit</t>
   </si>
   <si>
@@ -407,21 +287,12 @@
     <t>How many celsius</t>
   </si>
   <si>
-    <t>{answer1} celsius is {result} fahrenheit</t>
-  </si>
-  <si>
     <t>age in months</t>
   </si>
   <si>
     <t>How many years old are you?</t>
   </si>
   <si>
-    <t>You are {result} months old</t>
-  </si>
-  <si>
-    <t>Calculation</t>
-  </si>
-  <si>
     <t>{variable1} * {variable2}</t>
   </si>
   <si>
@@ -503,7 +374,214 @@
     <t>3.14 * {variable1} * {variable1}</t>
   </si>
   <si>
-    <t>The circle has an area of {result}</t>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>variable1</t>
+  </si>
+  <si>
+    <t>variable2</t>
+  </si>
+  <si>
+    <t>variable3</t>
+  </si>
+  <si>
+    <t>question1</t>
+  </si>
+  <si>
+    <t>question2</t>
+  </si>
+  <si>
+    <t>answer1</t>
+  </si>
+  <si>
+    <t>answer2</t>
+  </si>
+  <si>
+    <t>calculation</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>hours_practiced</t>
+  </si>
+  <si>
+    <t>age_in_ten</t>
+  </si>
+  <si>
+    <t>age_next_year</t>
+  </si>
+  <si>
+    <t>age_last_year</t>
+  </si>
+  <si>
+    <t>slices_left</t>
+  </si>
+  <si>
+    <t>each_owe</t>
+  </si>
+  <si>
+    <t>weight_kg</t>
+  </si>
+  <si>
+    <t>fits_in</t>
+  </si>
+  <si>
+    <t>remainder</t>
+  </si>
+  <si>
+    <t>months_to_save</t>
+  </si>
+  <si>
+    <t>daily_spend</t>
+  </si>
+  <si>
+    <t>total_spend</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>perimeter</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>difference</t>
+  </si>
+  <si>
+    <t>cookie_boxes</t>
+  </si>
+  <si>
+    <t>total_cycled</t>
+  </si>
+  <si>
+    <t>square</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>triple</t>
+  </si>
+  <si>
+    <t>fahrenheit</t>
+  </si>
+  <si>
+    <t>age_years</t>
+  </si>
+  <si>
+    <t>age_months</t>
+  </si>
+  <si>
+    <t>"Squidward has practiced", {result}, "hours"</t>
+  </si>
+  <si>
+    <t>{answer1}, "+", {answer2}, "is", {result}</t>
+  </si>
+  <si>
+    <t>{answer1}, "*", {answer2}, "is", {result}</t>
+  </si>
+  <si>
+    <t>{answer1}, "/", {answer2}, "is", {result}</t>
+  </si>
+  <si>
+    <t>{answer1}, "-", {answer2}, "is", {result}</t>
+  </si>
+  <si>
+    <t>"In 10 years, you will be", {result}</t>
+  </si>
+  <si>
+    <t>"Next year, you'll be", {result}</t>
+  </si>
+  <si>
+    <t>"Last year, you were", {result}</t>
+  </si>
+  <si>
+    <t>"You have", {result}, "slices left"</t>
+  </si>
+  <si>
+    <t>"You each owe £", {result}</t>
+  </si>
+  <si>
+    <t>{answer1}, "lbs is", {result}, "kg"</t>
+  </si>
+  <si>
+    <t>"There are", {result}, {answer2},"s in", {answer1}</t>
+  </si>
+  <si>
+    <t>"There are", {result}, "left over after dividing", {answer1}, "by", {answer2}</t>
+  </si>
+  <si>
+    <t>"There are", {result}, "hours in", {answer1}, "days"</t>
+  </si>
+  <si>
+    <t>{answer1}, "chocolate bars is", {result}</t>
+  </si>
+  <si>
+    <t>"You will have £", {result}, "a day"</t>
+  </si>
+  <si>
+    <t>"The area of the rectangle is", {result}</t>
+  </si>
+  <si>
+    <t>"The perimeter of the rectangle is", {result}</t>
+  </si>
+  <si>
+    <t>"There are", {result}, "seconds in", {answer1}, "minutes"</t>
+  </si>
+  <si>
+    <t>"The average is", {result}</t>
+  </si>
+  <si>
+    <t>"Person 1 is", {result}, "years older"</t>
+  </si>
+  <si>
+    <t>{answer1}, "needs", {result}, "boxes"</t>
+  </si>
+  <si>
+    <t>"You cycled", {result}, "km in", {answer2}, "days"</t>
+  </si>
+  <si>
+    <t>{answer1}, "squared is", {result}</t>
+  </si>
+  <si>
+    <t>"Half of", {answer1}, "is", {result}</t>
+  </si>
+  <si>
+    <t>"Double", {answer1}, "is", {result}</t>
+  </si>
+  <si>
+    <t>"The square is", {result}, "cm2"</t>
+  </si>
+  <si>
+    <t>"Triple", {answer1}, "is", {result}</t>
+  </si>
+  <si>
+    <t>{answer1}, "celsius is", {result}, "fahrenheit"</t>
+  </si>
+  <si>
+    <t>"You are", {result}, "months old"</t>
+  </si>
+  <si>
+    <t>"The circle has an area of", {result}</t>
+  </si>
+  <si>
+    <t>"It will take", {result}, "weeks to save ", {answer2}</t>
+  </si>
+  <si>
+    <t>How many hours a day has Squidward practiced?</t>
   </si>
 </sst>
 </file>
@@ -890,7 +968,7 @@
   <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K34" sqref="A1:K34"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -906,57 +984,57 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>118</v>
       </c>
       <c r="H1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
       <c r="K1" t="s">
-        <v>1</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="G2">
         <v>4</v>
@@ -965,33 +1043,33 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="J2">
         <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1000,33 +1078,33 @@
         <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="J3">
         <v>13</v>
       </c>
       <c r="K3" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -1035,33 +1113,33 @@
         <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="J4">
         <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1070,33 +1148,33 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="J5">
         <v>0.5</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G6">
         <v>10</v>
@@ -1105,111 +1183,111 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="J6">
         <v>6</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G7">
         <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="J7" s="1">
         <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="J8">
         <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G9">
         <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="J9">
         <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>8</v>
@@ -1218,33 +1296,33 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="J10">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -1253,59 +1331,59 @@
         <v>2</v>
       </c>
       <c r="I11" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="J11">
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="J12">
         <v>4.5</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G13">
         <v>20</v>
@@ -1314,33 +1392,33 @@
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="J13">
         <v>6</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>131</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G14">
         <v>20</v>
@@ -1349,59 +1427,59 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="J14">
         <v>2</v>
       </c>
       <c r="K14" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="G15">
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="J15">
         <v>120</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="G16" s="2">
         <v>30</v>
@@ -1410,33 +1488,33 @@
         <v>150</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="J16">
         <v>5</v>
       </c>
       <c r="K16" t="s">
-        <v>55</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="F17" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -1445,33 +1523,33 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="J17">
         <v>10</v>
       </c>
       <c r="K17" t="s">
-        <v>75</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -1480,33 +1558,33 @@
         <v>5</v>
       </c>
       <c r="I18" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="J18">
         <v>10</v>
       </c>
       <c r="K18" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="F19" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G19">
         <v>25</v>
@@ -1515,33 +1593,33 @@
         <v>5</v>
       </c>
       <c r="I19" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="J19">
         <v>125</v>
       </c>
       <c r="K19" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="F20" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G20">
         <v>25</v>
@@ -1550,59 +1628,59 @@
         <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="J20">
         <v>60</v>
       </c>
       <c r="K20" t="s">
-        <v>107</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="G21">
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="J21">
         <v>600</v>
       </c>
       <c r="K21" t="s">
-        <v>87</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>17</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -1611,33 +1689,33 @@
         <v>4</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="J22">
         <v>6</v>
       </c>
       <c r="K22" t="s">
-        <v>89</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="F23" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="G23">
         <v>15</v>
@@ -1646,33 +1724,33 @@
         <v>13</v>
       </c>
       <c r="I23" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="J23">
         <v>2</v>
       </c>
       <c r="K23" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="G24">
         <v>40</v>
@@ -1681,33 +1759,33 @@
         <v>5</v>
       </c>
       <c r="I24" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="J24">
         <v>8</v>
       </c>
       <c r="K24" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="G25">
         <v>50</v>
@@ -1716,247 +1794,247 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="J25">
         <v>150</v>
       </c>
       <c r="K25" t="s">
-        <v>106</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>10</v>
       </c>
       <c r="I26" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="J27">
         <v>10</v>
       </c>
       <c r="K27" t="s">
-        <v>111</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>144</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>20</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
       <c r="J28">
         <v>40</v>
       </c>
       <c r="K28" t="s">
-        <v>113</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="G29">
         <v>5</v>
       </c>
       <c r="I29" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="J29">
         <v>25</v>
       </c>
       <c r="K29" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="E30" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="G30">
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="J30">
         <v>16</v>
       </c>
       <c r="K30" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>20</v>
       </c>
       <c r="I31" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="J31">
         <v>60</v>
       </c>
       <c r="K31" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>146</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="G32">
         <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="J32">
         <v>86</v>
       </c>
       <c r="K32" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>148</v>
       </c>
       <c r="E33" t="s">
-        <v>125</v>
+        <v>84</v>
       </c>
       <c r="G33">
         <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="J33">
         <v>180</v>
       </c>
       <c r="K33" t="s">
-        <v>126</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="G34">
         <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="J34">
         <v>78.5</v>
       </c>
       <c r="K34" t="s">
-        <v>155</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>